<commit_message>
Got basic game working
</commit_message>
<xml_diff>
--- a/data/gamecorg.xlsx
+++ b/data/gamecorg.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="224">
   <si>
     <t>Halloween</t>
   </si>
@@ -54,6 +54,321 @@
     <t>Pamela Voorhees</t>
   </si>
   <si>
+    <t>Camp Crystal Lake</t>
+  </si>
+  <si>
+    <t>A Nightmare on Elm Street</t>
+  </si>
+  <si>
+    <t>Freddie Krueger</t>
+  </si>
+  <si>
+    <t>Nancy Thompson</t>
+  </si>
+  <si>
+    <t>Wes Craven</t>
+  </si>
+  <si>
+    <t>Heather Langenkamp</t>
+  </si>
+  <si>
+    <t>Robert Englund</t>
+  </si>
+  <si>
+    <t>The Shining</t>
+  </si>
+  <si>
+    <t>Stanley Kubrick</t>
+  </si>
+  <si>
+    <t>Jack Nicholson</t>
+  </si>
+  <si>
+    <t>Jack Torrance</t>
+  </si>
+  <si>
+    <t>Shelley Duvall</t>
+  </si>
+  <si>
+    <t>Wendy Torrance</t>
+  </si>
+  <si>
+    <t>Danny Torrance</t>
+  </si>
+  <si>
+    <t>Dick Hallorann</t>
+  </si>
+  <si>
+    <t>The Exorcist</t>
+  </si>
+  <si>
+    <t>William Peter Blatty</t>
+  </si>
+  <si>
+    <t>Linda Blair</t>
+  </si>
+  <si>
+    <t>Regan MacnNeil</t>
+  </si>
+  <si>
+    <t>Father Karras</t>
+  </si>
+  <si>
+    <t>Scream</t>
+  </si>
+  <si>
+    <t>Kevin Williamson</t>
+  </si>
+  <si>
+    <t>Courtney Cox</t>
+  </si>
+  <si>
+    <t>Neve campbell</t>
+  </si>
+  <si>
+    <t>David Arquette</t>
+  </si>
+  <si>
+    <t>Ghostface</t>
+  </si>
+  <si>
+    <t>Sidney Prescott</t>
+  </si>
+  <si>
+    <t>Gale Weathers</t>
+  </si>
+  <si>
+    <t>Dewey Riley</t>
+  </si>
+  <si>
+    <t>Candyman</t>
+  </si>
+  <si>
+    <t>Clive Barker</t>
+  </si>
+  <si>
+    <t>Tony Todd</t>
+  </si>
+  <si>
+    <t>Hellraiser</t>
+  </si>
+  <si>
+    <t>Cenobites</t>
+  </si>
+  <si>
+    <t>Pinhead</t>
+  </si>
+  <si>
+    <t>It Follows</t>
+  </si>
+  <si>
+    <t>The Strangers</t>
+  </si>
+  <si>
+    <t>The Mist</t>
+  </si>
+  <si>
+    <t>The Fog</t>
+  </si>
+  <si>
+    <t>The Thing</t>
+  </si>
+  <si>
+    <t>The Ring</t>
+  </si>
+  <si>
+    <t>Saw</t>
+  </si>
+  <si>
+    <t>Trick 'r Treat</t>
+  </si>
+  <si>
+    <t>American Psycho</t>
+  </si>
+  <si>
+    <t>The Silence of the Lambs</t>
+  </si>
+  <si>
+    <t>Hannibal Lecter</t>
+  </si>
+  <si>
+    <t>Clarice Starling</t>
+  </si>
+  <si>
+    <t>Gremlins</t>
+  </si>
+  <si>
+    <t>Alien</t>
+  </si>
+  <si>
+    <t>Ridley Scott</t>
+  </si>
+  <si>
+    <t>Siourney Weaver</t>
+  </si>
+  <si>
+    <t>Ripley</t>
+  </si>
+  <si>
+    <t>Black Christmas</t>
+  </si>
+  <si>
+    <t>Nope</t>
+  </si>
+  <si>
+    <t>Midsommar</t>
+  </si>
+  <si>
+    <t>Hereditary</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Pearl</t>
+  </si>
+  <si>
+    <t>Us</t>
+  </si>
+  <si>
+    <t>Get Out</t>
+  </si>
+  <si>
+    <t>A Quiet Place</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>Pennywise</t>
+  </si>
+  <si>
+    <t>Jeepers Creepers</t>
+  </si>
+  <si>
+    <t>Freaky</t>
+  </si>
+  <si>
+    <t>Urban Legend</t>
+  </si>
+  <si>
+    <t>Cabin in the Woods</t>
+  </si>
+  <si>
+    <t>Suspiria</t>
+  </si>
+  <si>
+    <t>Sleepaway Camp</t>
+  </si>
+  <si>
+    <t>Child's Play</t>
+  </si>
+  <si>
+    <t>Chucky</t>
+  </si>
+  <si>
+    <t>Unfriended</t>
+  </si>
+  <si>
+    <t>Happy Death Day</t>
+  </si>
+  <si>
+    <t>Ready or Not</t>
+  </si>
+  <si>
+    <t>You're Next</t>
+  </si>
+  <si>
+    <t>The Witch</t>
+  </si>
+  <si>
+    <t>As Above So Below</t>
+  </si>
+  <si>
+    <t>Final Girls</t>
+  </si>
+  <si>
+    <t>Krampus</t>
+  </si>
+  <si>
+    <t>The Visit</t>
+  </si>
+  <si>
+    <t>The Babadook</t>
+  </si>
+  <si>
+    <t>The Lighthouse</t>
+  </si>
+  <si>
+    <t>Lights Out</t>
+  </si>
+  <si>
+    <t>Sinister</t>
+  </si>
+  <si>
+    <t>The Conjuring</t>
+  </si>
+  <si>
+    <t>Insidious</t>
+  </si>
+  <si>
+    <t>Fresh</t>
+  </si>
+  <si>
+    <t>Green Room</t>
+  </si>
+  <si>
+    <t>Doctor Sleep</t>
+  </si>
+  <si>
+    <t>Saint Maud</t>
+  </si>
+  <si>
+    <t>The Love Witch</t>
+  </si>
+  <si>
+    <t>The Purge</t>
+  </si>
+  <si>
+    <t>Lake Mungo</t>
+  </si>
+  <si>
+    <t>The Blair Witch Project</t>
+  </si>
+  <si>
+    <t>Paranormal Activity</t>
+  </si>
+  <si>
+    <t>Pet Sematary</t>
+  </si>
+  <si>
+    <t>Christine</t>
+  </si>
+  <si>
+    <t>Silent Hill</t>
+  </si>
+  <si>
+    <t>Resident Evil</t>
+  </si>
+  <si>
+    <t>Dawn of the Dead</t>
+  </si>
+  <si>
+    <t>Night of the Living Dead</t>
+  </si>
+  <si>
+    <t>John Romero</t>
+  </si>
+  <si>
+    <t>The Lost Boys</t>
+  </si>
+  <si>
+    <t>Fear Street</t>
+  </si>
+  <si>
+    <t>Misery</t>
+  </si>
+  <si>
     <t>Frodo Baggins</t>
   </si>
   <si>
@@ -87,6 +402,96 @@
     <t>Ian McKellen</t>
   </si>
   <si>
+    <t>Gollum</t>
+  </si>
+  <si>
+    <t>Andy Serkis</t>
+  </si>
+  <si>
+    <t>Riders of Rohan</t>
+  </si>
+  <si>
+    <t>Balrog</t>
+  </si>
+  <si>
+    <t>Mines of Moria</t>
+  </si>
+  <si>
+    <t>Elves</t>
+  </si>
+  <si>
+    <t>Dwarves</t>
+  </si>
+  <si>
+    <t>Hobbits</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Isildur</t>
+  </si>
+  <si>
+    <t>Boromir</t>
+  </si>
+  <si>
+    <t>Denethor</t>
+  </si>
+  <si>
+    <t>Saruman</t>
+  </si>
+  <si>
+    <t>Christopher Lee</t>
+  </si>
+  <si>
+    <t>Gimli</t>
+  </si>
+  <si>
+    <t>Arwen</t>
+  </si>
+  <si>
+    <t>Faramir</t>
+  </si>
+  <si>
+    <t>Witch-king of Angmar</t>
+  </si>
+  <si>
+    <t>Ringwraiths</t>
+  </si>
+  <si>
+    <t>Grima Wormtongue</t>
+  </si>
+  <si>
+    <t>Galadriel</t>
+  </si>
+  <si>
+    <t>Pippin</t>
+  </si>
+  <si>
+    <t>Merry</t>
+  </si>
+  <si>
+    <t>Ents</t>
+  </si>
+  <si>
+    <t>Treebeard</t>
+  </si>
+  <si>
+    <t>Sauron</t>
+  </si>
+  <si>
+    <t>Elrond</t>
+  </si>
+  <si>
+    <t>Theoden</t>
+  </si>
+  <si>
+    <t>Smaug</t>
+  </si>
+  <si>
+    <t>Benedict Cumberbatch</t>
+  </si>
+  <si>
     <t>Luke Skywalker</t>
   </si>
   <si>
@@ -121,6 +526,165 @@
   </si>
   <si>
     <t>George Lucas</t>
+  </si>
+  <si>
+    <t>Wookies</t>
+  </si>
+  <si>
+    <t>Boba Fett</t>
+  </si>
+  <si>
+    <t>Anakin Skywalker</t>
+  </si>
+  <si>
+    <t>Obi-Wan Kenobi</t>
+  </si>
+  <si>
+    <t>Ewan McGregor</t>
+  </si>
+  <si>
+    <t>Bail Organa</t>
+  </si>
+  <si>
+    <t>Tatooine</t>
+  </si>
+  <si>
+    <t>Hoth</t>
+  </si>
+  <si>
+    <t>Mustafar</t>
+  </si>
+  <si>
+    <t>Coruscant</t>
+  </si>
+  <si>
+    <t>Alderaan</t>
+  </si>
+  <si>
+    <t>Kashkyyyk</t>
+  </si>
+  <si>
+    <t>Naboo</t>
+  </si>
+  <si>
+    <t>Kamino</t>
+  </si>
+  <si>
+    <t>Bespin</t>
+  </si>
+  <si>
+    <t>Palpatine</t>
+  </si>
+  <si>
+    <t>Darth Sidious</t>
+  </si>
+  <si>
+    <t>Darth Maul</t>
+  </si>
+  <si>
+    <t>Count Dooku</t>
+  </si>
+  <si>
+    <t>Yoda</t>
+  </si>
+  <si>
+    <t>Younglings</t>
+  </si>
+  <si>
+    <t>Podracing</t>
+  </si>
+  <si>
+    <t>Grand Moff Tarkin</t>
+  </si>
+  <si>
+    <t>Jar Jar Binks</t>
+  </si>
+  <si>
+    <t>Vice-Admiral Holdo</t>
+  </si>
+  <si>
+    <t>Salacious B. Crumb</t>
+  </si>
+  <si>
+    <t>Wicket</t>
+  </si>
+  <si>
+    <t>Ewoks</t>
+  </si>
+  <si>
+    <t>Sebulba</t>
+  </si>
+  <si>
+    <t>Wedge Antilles</t>
+  </si>
+  <si>
+    <t>Finn</t>
+  </si>
+  <si>
+    <t>Rey</t>
+  </si>
+  <si>
+    <t>Poe Dameron</t>
+  </si>
+  <si>
+    <t>Jabba the Hutt</t>
+  </si>
+  <si>
+    <t>Mon Mothma</t>
+  </si>
+  <si>
+    <t>Smuggler</t>
+  </si>
+  <si>
+    <t>Bounty Hunter</t>
+  </si>
+  <si>
+    <t>The Mandalorian</t>
+  </si>
+  <si>
+    <t>Cassian Andor</t>
+  </si>
+  <si>
+    <t>Jyn Erso</t>
+  </si>
+  <si>
+    <t>Saw Gerrera</t>
+  </si>
+  <si>
+    <t>The Phantom Menace</t>
+  </si>
+  <si>
+    <t>Attack of the Clones</t>
+  </si>
+  <si>
+    <t>Revenge of the Sith</t>
+  </si>
+  <si>
+    <t>A New Hope</t>
+  </si>
+  <si>
+    <t>The Empire Strikes Back</t>
+  </si>
+  <si>
+    <t>Return of the Jedi</t>
+  </si>
+  <si>
+    <t>The Force Awakens</t>
+  </si>
+  <si>
+    <t>The Last Jedi</t>
+  </si>
+  <si>
+    <t>The Rise of Skywalker</t>
+  </si>
+  <si>
+    <t>Solo</t>
+  </si>
+  <si>
+    <t>Rogue One</t>
+  </si>
+  <si>
+    <t>Millenium Falcon</t>
   </si>
 </sst>
 </file>
@@ -453,6 +1017,531 @@
         <v>12</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -470,57 +1559,212 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -543,62 +1787,332 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted old app.js file
</commit_message>
<xml_diff>
--- a/data/gamecorg.xlsx
+++ b/data/gamecorg.xlsx
@@ -246,7 +246,7 @@
     <t>Patsy Tacos</t>
   </si>
   <si>
-    <t>Tom's Baked Beans</t>
+    <t>Toms Baked Beans</t>
   </si>
   <si>
     <t>Rae</t>
@@ -258,7 +258,7 @@
     <t>Luminaria</t>
   </si>
   <si>
-    <t>Haley's David</t>
+    <t>Haleys David</t>
   </si>
   <si>
     <t>Cameron</t>
@@ -279,7 +279,7 @@
     <t>Safeway</t>
   </si>
   <si>
-    <t>Sun's Teriyaki</t>
+    <t>Suns Teriyaki</t>
   </si>
   <si>
     <t>Seahawks</t>
@@ -309,7 +309,7 @@
     <t>BYU</t>
   </si>
   <si>
-    <t>BYU-Idaho</t>
+    <t>BYU Idaho</t>
   </si>
   <si>
     <t>Southern Utah University</t>
@@ -336,7 +336,7 @@
     <t>University of New Mexico</t>
   </si>
   <si>
-    <t>Everybody's a Lobo</t>
+    <t>Everybodys a Lobo</t>
   </si>
   <si>
     <t>Do you want it or not?</t>
@@ -411,7 +411,7 @@
     <t>Janice Lunt</t>
   </si>
   <si>
-    <t>Megan's Megans</t>
+    <t>Megans Megans</t>
   </si>
   <si>
     <t>Shon Lunt</t>
@@ -420,7 +420,7 @@
     <t>Chantel Bills</t>
   </si>
   <si>
-    <t>Dad's friend Mike</t>
+    <t>Dads friend Mike</t>
   </si>
   <si>
     <t>Mitch Smith</t>
@@ -645,7 +645,7 @@
     <t>Saw</t>
   </si>
   <si>
-    <t>Trick 'r Treat</t>
+    <t>Trick r Treat</t>
   </si>
   <si>
     <t>American Psycho</t>
@@ -726,7 +726,7 @@
     <t>Sleepaway Camp</t>
   </si>
   <si>
-    <t>Child's Play</t>
+    <t>Childs Play</t>
   </si>
   <si>
     <t>Chucky</t>
@@ -741,7 +741,7 @@
     <t>Ready or Not</t>
   </si>
   <si>
-    <t>You're Next</t>
+    <t>Youre Next</t>
   </si>
   <si>
     <t>The Witch</t>
@@ -834,7 +834,7 @@
     <t>Misery</t>
   </si>
   <si>
-    <t>Jennifer's Body</t>
+    <t>Jennifers Body</t>
   </si>
   <si>
     <t>The Fly</t>
@@ -1353,7 +1353,7 @@
     <t>What about the droid attack on the wookies?</t>
   </si>
   <si>
-    <t>Well I don't approve</t>
+    <t>Well I dont approve</t>
   </si>
   <si>
     <t>Now this is podracing!</t>
@@ -1410,10 +1410,10 @@
     <t>General Kenobi</t>
   </si>
   <si>
-    <t>I don't like sand.</t>
-  </si>
-  <si>
-    <t>It's course and rough and irritating</t>
+    <t>I dont like sand.</t>
+  </si>
+  <si>
+    <t>Its course and rough and irritating</t>
   </si>
   <si>
     <t>Are you an angel?</t>
@@ -1425,7 +1425,7 @@
     <t>Watto</t>
   </si>
   <si>
-    <t>Bad bombin'</t>
+    <t>Bad bombin</t>
   </si>
   <si>
     <t>Then you are Lost!</t>
@@ -1491,7 +1491,7 @@
     <t>Visible confusion</t>
   </si>
   <si>
-    <t>That's why I'm here</t>
+    <t>Thats why Im here</t>
   </si>
   <si>
     <t>Rian Johnson</t>
@@ -1632,7 +1632,7 @@
     <t>Probe Droid</t>
   </si>
   <si>
-    <t>It's an older code sir, but it checks out</t>
+    <t>Its an older code sir, but it checks out</t>
   </si>
   <si>
     <t>Luke</t>
@@ -1671,7 +1671,7 @@
     <t>Uaeb</t>
   </si>
   <si>
-    <t>Eznog's Eggnog</t>
+    <t>Eznogs Eggnog</t>
   </si>
   <si>
     <t>Send your little angel home early</t>
@@ -1821,7 +1821,7 @@
     <t>Ulysses</t>
   </si>
   <si>
-    <t>Beau's PBS show</t>
+    <t>Beaus PBS show</t>
   </si>
   <si>
     <t>Mormon</t>
@@ -2055,7 +2055,7 @@
     <t>Pepper Poppers</t>
   </si>
   <si>
-    <t>Miner's Treat</t>
+    <t>Miners Treat</t>
   </si>
   <si>
     <t>Triple Shot Espresso</t>
@@ -2376,7 +2376,7 @@
     <t>Tammy Swanson</t>
   </si>
   <si>
-    <t>Lil' Sebastian</t>
+    <t>Lil Sebastian</t>
   </si>
   <si>
     <t>Burt Macklin</t>
@@ -2388,7 +2388,7 @@
     <t>Calzones</t>
   </si>
   <si>
-    <t>Tom's Bistro</t>
+    <t>Toms Bistro</t>
   </si>
   <si>
     <t>City Hall</t>
@@ -2397,7 +2397,7 @@
     <t>Waffles</t>
   </si>
   <si>
-    <t>JJ's Diner</t>
+    <t>JJs Diner</t>
   </si>
   <si>
     <t>Cones of Dunshire</t>
@@ -2550,7 +2550,7 @@
     <t>Frozen Banana Stand</t>
   </si>
   <si>
-    <t>There's always money in the banana stand</t>
+    <t>Theres always money in the banana stand</t>
   </si>
   <si>
     <t>I love Marta</t>
@@ -2589,7 +2589,7 @@
     <t>Gene Parmesan</t>
   </si>
   <si>
-    <t>He's going to be all right</t>
+    <t>Hes going to be all right</t>
   </si>
   <si>
     <t>Loose seal</t>
@@ -2598,7 +2598,7 @@
     <t>Don Quixote</t>
   </si>
   <si>
-    <t>Alice's Adventures in Wonderland</t>
+    <t>Alices Adventures in Wonderland</t>
   </si>
   <si>
     <t>The Adventures of Huckleberry Finn</t>
@@ -2625,10 +2625,10 @@
     <t>The Scarlet Letter</t>
   </si>
   <si>
-    <t>Gulliver's Travels</t>
-  </si>
-  <si>
-    <t>The Pilgrim's Progress</t>
+    <t>Gullivers Travels</t>
+  </si>
+  <si>
+    <t>The Pilgrims Progress</t>
   </si>
   <si>
     <t>A Christmas Carol</t>
@@ -2655,7 +2655,7 @@
     <t>Oliver Twist</t>
   </si>
   <si>
-    <t>Uncle Tom's Cabin</t>
+    <t>Uncle Toms Cabin</t>
   </si>
   <si>
     <t>Crime and Punishment</t>
@@ -2721,10 +2721,10 @@
     <t>The Last of the Mohicans</t>
   </si>
   <si>
-    <t>Tess of the d'Urbervilles</t>
-  </si>
-  <si>
-    <t>Harry Potter and the Sorcerer's Stone</t>
+    <t>Tess of the dUrbervilles</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Sorcerers Stone</t>
   </si>
   <si>
     <t>Heidi</t>
@@ -2796,7 +2796,7 @@
     <t>The Trial</t>
   </si>
   <si>
-    <t>Lady Chatterley's Lover</t>
+    <t>Lady Chatterleys Lover</t>
   </si>
   <si>
     <t>Kidnapped: The Adventures of David Balfour</t>
@@ -2829,7 +2829,7 @@
     <t>The Vicar of Wakefield</t>
   </si>
   <si>
-    <t>A Connecticut Yankee in King Arthur's Court</t>
+    <t>A Connecticut Yankee in King Arthurs Court</t>
   </si>
   <si>
     <t>White Fang</t>
@@ -2877,7 +2877,7 @@
     <t>Sons and Lovers</t>
   </si>
   <si>
-    <t>Charlotte's Web</t>
+    <t>Charlottes Web</t>
   </si>
   <si>
     <t>The Swiss Family Robinson</t>
@@ -2958,7 +2958,7 @@
     <t>To the Lighthouse</t>
   </si>
   <si>
-    <t>The Magician's Nephew</t>
+    <t>The Magicians Nephew</t>
   </si>
   <si>
     <t>Harry Potter and the Order of the Phoenix</t>
@@ -3024,7 +3024,7 @@
     <t>The Kite Runner</t>
   </si>
   <si>
-    <t>One Flew Over the Cuckoo's Nest</t>
+    <t>One Flew Over the Cuckoos Nest</t>
   </si>
   <si>
     <t>The Portrait of a Lady</t>
@@ -3081,7 +3081,7 @@
     <t>O Pioneers!</t>
   </si>
   <si>
-    <t>The Handmaid's Tale</t>
+    <t>The Handmaids Tale</t>
   </si>
   <si>
     <t>The Moonstone</t>
@@ -3267,7 +3267,7 @@
     <t>The Red Pony</t>
   </si>
   <si>
-    <t>All the King's Men</t>
+    <t>All the Kings Men</t>
   </si>
   <si>
     <t>Things Fall Apart</t>
@@ -3366,7 +3366,7 @@
     <t>Sounder</t>
   </si>
   <si>
-    <t>Are You There God? It's Me, Margaret</t>
+    <t>Are You There God? Its Me, Margaret</t>
   </si>
   <si>
     <t>The Notebook</t>
@@ -3387,10 +3387,10 @@
     <t>The Firm</t>
   </si>
   <si>
-    <t>Swann's Way</t>
-  </si>
-  <si>
-    <t>Ender's Game</t>
+    <t>Swanns Way</t>
+  </si>
+  <si>
+    <t>Enders Game</t>
   </si>
   <si>
     <t>The Name of the Rose</t>
@@ -3408,7 +3408,7 @@
     <t>Eragon</t>
   </si>
   <si>
-    <t>The Hitchhiker's Guide to the Galaxy</t>
+    <t>The Hitchhikers Guide to the Galaxy</t>
   </si>
   <si>
     <t>Buddenbrooks</t>
@@ -3438,7 +3438,7 @@
     <t>Where the Red Fern Grows</t>
   </si>
   <si>
-    <t>Le Morte D'Arthur</t>
+    <t>Le Morte DArthur</t>
   </si>
   <si>
     <t>Mockingjay</t>
@@ -3573,7 +3573,7 @@
     <t>The Tale of Despereaux</t>
   </si>
   <si>
-    <t>The Girl Who Kicked the Hornet's Nest</t>
+    <t>The Girl Who Kicked the Hornets Nest</t>
   </si>
   <si>
     <t>Dear Mr. Henshaw</t>
@@ -3597,7 +3597,7 @@
     <t>P Is for Peril</t>
   </si>
   <si>
-    <t>My Sister's Keeper</t>
+    <t>My Sisters Keeper</t>
   </si>
   <si>
     <t>Barnaby Rudge</t>
@@ -3696,7 +3696,7 @@
     <t>Inferno</t>
   </si>
   <si>
-    <t>Schindler's List</t>
+    <t>Schindlers List</t>
   </si>
   <si>
     <t>Jonathan Livingston Seagull</t>
@@ -3738,7 +3738,7 @@
     <t>Encyclopedia Brown: Boy Detective</t>
   </si>
   <si>
-    <t>The Time Traveler's Wife</t>
+    <t>The Time Travelers Wife</t>
   </si>
   <si>
     <t>The Incredible Journey</t>
@@ -3813,7 +3813,7 @@
     <t>Diary of a Wimpy Kid: The Last Straw</t>
   </si>
   <si>
-    <t>King Solomon's Mines</t>
+    <t>King Solomons Mines</t>
   </si>
   <si>
     <t>The Princess of Cleves</t>
@@ -3900,7 +3900,7 @@
     <t>The Fall</t>
   </si>
   <si>
-    <t>The No. 1 Ladies' Detective Agency</t>
+    <t>The No. 1 Ladies Detective Agency</t>
   </si>
   <si>
     <t>Worst Case</t>
@@ -3933,22 +3933,22 @@
     <t>Walk Two Moons</t>
   </si>
   <si>
-    <t>Miss Peregrine's Home for Peculiar Children</t>
+    <t>Miss Peregrines Home for Peculiar Children</t>
   </si>
   <si>
     <t>The Chocolate War</t>
   </si>
   <si>
-    <t>Sophie's Choice</t>
+    <t>Sophies Choice</t>
   </si>
   <si>
     <t>Looking for Alaska</t>
   </si>
   <si>
-    <t>Breakfast at Tiffany's</t>
-  </si>
-  <si>
-    <t>The Razor's Edge</t>
+    <t>Breakfast at Tiffanys</t>
+  </si>
+  <si>
+    <t>The Razors Edge</t>
   </si>
   <si>
     <t>Dreamcatcher</t>
@@ -3978,7 +3978,7 @@
     <t>Diary of a Wimpy Kid</t>
   </si>
   <si>
-    <t>The Memory Keeper's Daughter</t>
+    <t>The Memory Keepers Daughter</t>
   </si>
   <si>
     <t>The Wedding</t>
@@ -3999,7 +3999,7 @@
     <t>The Death of Ivan Ilych</t>
   </si>
   <si>
-    <t>Alex Cross's Trial</t>
+    <t>Alex Crosss Trial</t>
   </si>
   <si>
     <t>Kenilworth</t>
@@ -4029,7 +4029,7 @@
     <t>Swimsuit</t>
   </si>
   <si>
-    <t>Cat's Cradle</t>
+    <t>Cats Cradle</t>
   </si>
   <si>
     <t>The Caine Mutiny</t>
@@ -4302,7 +4302,7 @@
     <t>George Eliot</t>
   </si>
   <si>
-    <t>Madeleine L'Engle</t>
+    <t>Madeleine LEngle</t>
   </si>
   <si>
     <t>H.G. Wells</t>
@@ -4797,7 +4797,7 @@
     <t>Madame de (Marie-Madeleine Pioche de La Vergne) La Fayett</t>
   </si>
   <si>
-    <t>Robert C. O'Brien</t>
+    <t>Robert C. OBrien</t>
   </si>
   <si>
     <t>John Irving</t>
@@ -4854,7 +4854,7 @@
     <t>William Styron</t>
   </si>
   <si>
-    <t>Tim O'Brien</t>
+    <t>Tim OBrien</t>
   </si>
   <si>
     <t>Edwin A. Abbott</t>
@@ -4980,7 +4980,7 @@
     <t>Southpark</t>
   </si>
   <si>
-    <t>It's Always Sunny in Philadelphia</t>
+    <t>Its Always Sunny in Philadelphia</t>
   </si>
   <si>
     <t>Deadwood</t>
@@ -5097,7 +5097,7 @@
     <t>Once Upon a Time</t>
   </si>
   <si>
-    <t>Grey's Anatomy</t>
+    <t>Greys Anatomy</t>
   </si>
   <si>
     <t>Hannibal</t>
@@ -5295,7 +5295,7 @@
     <t>Yellowstone</t>
   </si>
   <si>
-    <t>Handmaid's Tale</t>
+    <t>Handmaids Tale</t>
   </si>
   <si>
     <t>American Gods</t>

</xml_diff>